<commit_message>
Add rotary switch doc, footprint, and basic circuit
</commit_message>
<xml_diff>
--- a/hardware/plans/v1_bom.xlsx
+++ b/hardware/plans/v1_bom.xlsx
@@ -328,13 +328,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -345,12 +347,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -686,7 +690,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Re-arrange switch connector pinout to simpler single-row header. Re-route the switch boards accordingly.
</commit_message>
<xml_diff>
--- a/hardware/plans/v1_bom.xlsx
+++ b/hardware/plans/v1_bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24500" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
   <si>
     <t>Quantity</t>
   </si>
@@ -196,9 +196,6 @@
     <t>flux laser studio glasgow</t>
   </si>
   <si>
-    <t>main board pcb production</t>
-  </si>
-  <si>
     <t>ragworm</t>
   </si>
   <si>
@@ -253,28 +250,70 @@
     <t>2.5A power supply for printer</t>
   </si>
   <si>
-    <t>Power supply for raspberry pi</t>
-  </si>
-  <si>
     <t>old telephone dial</t>
   </si>
   <si>
-    <t>regular HDMI screen for delay line display?</t>
-  </si>
-  <si>
     <t>ebay</t>
   </si>
   <si>
     <t>amazon</t>
   </si>
   <si>
-    <t>overall housing box/rack?</t>
-  </si>
-  <si>
-    <t>Extended Price</t>
-  </si>
-  <si>
-    <t>Total Cost</t>
+    <t>Total Cost inc VAT</t>
+  </si>
+  <si>
+    <t>Extended Price inc VAT</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Waveshare-Capacitive-Interface-Raspberry-Beaglebone/dp/B015E8EDYQ/ref=sr_1_3?ie=UTF8&amp;qid=1470731697&amp;sr=8-3&amp;keywords=7+inch+waveshare+lcd+c</t>
+  </si>
+  <si>
+    <t>7 inch HDMI display with mounting holes, could alternatively get a full size mnonitor</t>
+  </si>
+  <si>
+    <t>waveshare 7 inch LCD(C) 1024x600 Rev 2.1</t>
+  </si>
+  <si>
+    <t>2A Power supply for raspberry pi</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Aukru-Supply-Charger-Raspberry-Banana/dp/B017YW26YE/ref=sr_1_4?ie=UTF8&amp;qid=1470731884&amp;sr=8-4&amp;keywords=2a+power+supply+micro+usb</t>
+  </si>
+  <si>
+    <t>Aukru Micro USB Power Supply 5V 2000mA</t>
+  </si>
+  <si>
+    <t>AC/DC WALL MOUNT ADAPTER 5V 12W</t>
+  </si>
+  <si>
+    <t>1470-3108-ND</t>
+  </si>
+  <si>
+    <t>SC14012</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/SanDisk-Extreme-microSDHC-Frustration-Packaging/dp/B013P1M49A/ref=sr_1_1?ie=UTF8&amp;qid=1470732316&amp;sr=8-1&amp;keywords=16gb+micro+sd+sandisk+u3</t>
+  </si>
+  <si>
+    <t>SanDisk Extreme 16 GB microSDHC Class 10 </t>
+  </si>
+  <si>
+    <t>main board pcb production 100x100</t>
+  </si>
+  <si>
+    <t>mc slip button</t>
+  </si>
+  <si>
+    <t>SWITCH PUSH SPST-NO 3A 120V</t>
+  </si>
+  <si>
+    <t>EG1932-ND</t>
+  </si>
+  <si>
+    <t>Box / Rack for mounting front panel and main board in</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -311,12 +350,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -328,7 +373,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,14 +385,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -355,6 +404,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -687,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -728,7 +778,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -779,7 +829,7 @@
         <v>1.764</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F38" si="0">E3*1.2</f>
+        <f t="shared" ref="F3:F28" si="0">E3*1.2</f>
         <v>2.1168</v>
       </c>
       <c r="G3">
@@ -789,7 +839,7 @@
         <v>21</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I32" si="1">A3*F3</f>
+        <f t="shared" ref="I3:I49" si="1">A3*F3</f>
         <v>105.84</v>
       </c>
     </row>
@@ -1031,7 +1081,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -1054,7 +1104,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>0.84</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1154,7 +1204,7 @@
       <c r="A16">
         <v>20</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C16" t="s">
@@ -1179,7 +1229,7 @@
       <c r="A17">
         <v>20</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C17" t="s">
@@ -1272,19 +1322,22 @@
       <c r="C20" t="s">
         <v>53</v>
       </c>
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
       <c r="E20">
-        <v>29.99</v>
+        <v>25.99</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>35.988</v>
+        <v>31.187999999999995</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>35.988</v>
+        <v>31.187999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1308,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
@@ -1320,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="E22" t="s">
-        <v>72</v>
+      <c r="E22" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="F22">
         <v>50</v>
@@ -1335,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
@@ -1346,11 +1399,11 @@
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
         <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
       </c>
       <c r="F23">
         <v>40.299999999999997</v>
@@ -1359,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
@@ -1371,10 +1424,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>3.28</v>
@@ -1383,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
@@ -1395,13 +1448,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25">
         <v>3.46</v>
@@ -1414,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
@@ -1426,10 +1479,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
       </c>
       <c r="D26">
         <v>695</v>
@@ -1445,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
@@ -1457,10 +1510,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27">
         <v>696</v>
@@ -1484,18 +1537,31 @@
       <c r="A28">
         <v>1</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28">
+        <v>8.2200000000000006</v>
       </c>
       <c r="F28">
+        <f t="shared" si="0"/>
+        <v>9.8640000000000008</v>
+      </c>
+      <c r="G28">
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.8640000000000008</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1503,20 +1569,26 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>4.99</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1524,41 +1596,47 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
         <v>80</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>45.99</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>45.99</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F31">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1566,20 +1644,166 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
       </c>
       <c r="F32">
-        <v>15</v>
-      </c>
-      <c r="H32" t="s">
-        <v>77</v>
+        <v>8.42</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8.42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33">
+        <v>2.08</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F34" si="2">E33*1.2</f>
+        <v>2.496</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>2.496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9">
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1599,27 +1823,27 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
         <f>SUM(Sheet1!I:I)</f>
-        <v>586.56960000000004</v>
+        <v>584.36959999999988</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2" emptyCellReference="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add processed files ready for laser cutting.
</commit_message>
<xml_diff>
--- a/hardware/plans/v1_bom.xlsx
+++ b/hardware/plans/v1_bom.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32880" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -447,57 +447,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -835,10 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1253,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1288,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1323,7 +1274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1428,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1456,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1526,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1558,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1590,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1622,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1650,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1678,7 +1629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1713,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1748,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1815,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1846,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1877,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1905,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1971,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2000,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2013,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="I37">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2023,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="I38">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2033,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="I39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2043,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1">
       <c r="I40">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2053,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="I41">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2063,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1">
       <c r="I42">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2073,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="I43">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2083,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1">
       <c r="I44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2093,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="I45">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2103,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="I46">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="I47">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2123,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="I48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2133,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="9:10">
+    <row r="49" spans="9:10" hidden="1">
       <c r="I49">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2143,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="9:10">
+    <row r="50" spans="9:10" hidden="1">
       <c r="I50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2154,9 +2105,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F12"/>
+  <autoFilter ref="A1:F50">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="DIGIKEY"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct mistake on laser cutting file, add parts order list.
</commit_message>
<xml_diff>
--- a/hardware/plans/v1_bom.xlsx
+++ b/hardware/plans/v1_bom.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>Quantity</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Output: 5V 1A, for lights</t>
   </si>
   <si>
-    <t>AE40M-5-ND</t>
-  </si>
-  <si>
     <t>RAPID</t>
   </si>
   <si>
@@ -142,18 +139,9 @@
     <t>PCB production base material</t>
   </si>
   <si>
-    <t>MOSFET N-CH 60V 0.2A TO-92</t>
-  </si>
-  <si>
-    <t>2N7000TACT-ND</t>
-  </si>
-  <si>
     <t>mosfet for max7221 logic level shifter</t>
   </si>
   <si>
-    <t>CPC</t>
-  </si>
-  <si>
     <t>Raspberry Pi 3</t>
   </si>
   <si>
@@ -172,15 +160,6 @@
     <t>100x100mm double sided PCB guide price</t>
   </si>
   <si>
-    <t>B&amp;Q</t>
-  </si>
-  <si>
-    <t>M3 Screw and nut for holding LEDs in place</t>
-  </si>
-  <si>
-    <t>m3 screw 25mm and nut, pack of 10</t>
-  </si>
-  <si>
     <t>655-3235</t>
   </si>
   <si>
@@ -247,9 +226,6 @@
     <t>1470-3108-ND</t>
   </si>
   <si>
-    <t>SC14012</t>
-  </si>
-  <si>
     <t>https://www.amazon.co.uk/SanDisk-Extreme-microSDHC-Frustration-Packaging/dp/B013P1M49A/ref=sr_1_1?ie=UTF8&amp;qid=1470732316&amp;sr=8-1&amp;keywords=16gb+micro+sd+sandisk+u3</t>
   </si>
   <si>
@@ -338,13 +314,55 @@
   </si>
   <si>
     <t>one-shot dial tbd</t>
+  </si>
+  <si>
+    <t>160-1964-ND</t>
+  </si>
+  <si>
+    <t>LED RED DIFF 5MM ROUND T/H</t>
+  </si>
+  <si>
+    <t>alarum</t>
+  </si>
+  <si>
+    <t>39-0224</t>
+  </si>
+  <si>
+    <t>2n7000TA Fairchild (in pack of ten)</t>
+  </si>
+  <si>
+    <t>214-0661</t>
+  </si>
+  <si>
+    <t>http://www.amazon.co.uk/dp/B01CCOXV34</t>
+  </si>
+  <si>
+    <t>M3 x 20mm bolts</t>
+  </si>
+  <si>
+    <t>http://www.amazon.co.uk/dp/B00GYS1SXU</t>
+  </si>
+  <si>
+    <t>M3 hex nuts</t>
+  </si>
+  <si>
+    <t>http://www.amazon.co.uk/dp/B015A38FUS</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>cutting time</t>
+  </si>
+  <si>
+    <t>delivery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,8 +399,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +417,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -404,7 +446,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -420,8 +462,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -429,8 +498,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="15"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="42">
     <cellStyle name="Bad" xfId="14" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -442,12 +515,69 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="15" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -785,11 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I34"/>
+      <selection activeCell="I33" sqref="I33:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,907 +957,890 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1.514</v>
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1.2</f>
-        <v>1.8168</v>
+        <v>30.7</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>A2*F2</f>
-        <v>72.671999999999997</v>
+        <v>30.7</v>
       </c>
       <c r="J2">
         <f>MAX(0, A2-G2)</f>
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1.764</v>
+        <v>56</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F29" si="0">E3*1.2</f>
-        <v>2.1168</v>
+        <v>4.99</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I50" si="1">A3*F3</f>
-        <v>105.84</v>
+        <f>A3*F3</f>
+        <v>4.99</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J50" si="2">MAX(0, A3-G3)</f>
-        <v>49</v>
+        <f>MAX(0, A3-G3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.14</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5680000000000001</v>
+        <v>45.99</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
-        <v>7.7040000000000006</v>
+        <f>A4*F4</f>
+        <v>45.99</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A4-G4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.62</v>
+        <v>56</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>1.944</v>
+        <v>10.47</v>
       </c>
       <c r="G5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>5.8319999999999999</v>
+        <f>A5*F5</f>
+        <v>10.47</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A5-G5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.9</v>
+        <v>56</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.08</v>
+        <v>7.07</v>
       </c>
       <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
-        <v>12.96</v>
+        <f>A6*F6</f>
+        <v>7.07</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f>MAX(0, A6-G6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6.97</v>
+        <v>56</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>8.363999999999999</v>
+        <v>3.23</v>
       </c>
       <c r="G7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
-        <v>16.727999999999998</v>
+        <f>A7*F7</f>
+        <v>3.23</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A7-G7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>100</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="D8" s="7">
+        <v>695</v>
       </c>
       <c r="E8" s="1">
-        <v>0.2092</v>
+        <v>37.92</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.25103999999999999</v>
+        <f>E8*1.2</f>
+        <v>45.503999999999998</v>
       </c>
       <c r="G8" s="1">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
-        <v>25.103999999999999</v>
+        <f>A8*F8</f>
+        <v>45.503999999999998</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A8-G8)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
+      <c r="B9" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="D9" s="7">
+        <v>696</v>
       </c>
       <c r="E9" s="1">
-        <v>0.19</v>
+        <v>1.63</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.22799999999999998</v>
+        <f>E9*1.2</f>
+        <v>1.9559999999999997</v>
       </c>
       <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>A9*F9</f>
+        <v>3.9119999999999995</v>
+      </c>
+      <c r="J9">
+        <f>MAX(0, A9-G9)</f>
         <v>2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0.45599999999999996</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>0.22</v>
+        <v>1.514</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.26400000000000001</v>
+        <f>E10*1.2</f>
+        <v>1.8168</v>
       </c>
       <c r="G10" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>3.1680000000000001</v>
+        <f>A10*F10</f>
+        <v>72.671999999999997</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f>MAX(0, A10-G10)</f>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
+      <c r="D11" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="E11" s="1">
-        <v>4.71</v>
+        <v>1.764</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>5.6520000000000001</v>
+        <f>E11*1.2</f>
+        <v>2.1168</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
-        <v>5.6520000000000001</v>
+        <f>A11*F11</f>
+        <v>105.84</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A11-G11)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E12" s="1">
-        <v>0.7</v>
+        <v>2.14</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.84</v>
+        <f>E12*1.2</f>
+        <v>2.5680000000000001</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1.68</v>
+        <f>A12*F12</f>
+        <v>12.84</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>89</v>
+        <f>MAX(0, A12-G12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="10">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1">
-        <v>0.28999999999999998</v>
+        <v>1.62</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.34799999999999998</v>
+        <f>E13*1.2</f>
+        <v>1.944</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>4.1760000000000002</v>
+        <f>A13*F13</f>
+        <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1">
+        <f>MAX(0, A13-G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>87</v>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>17</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>0.23</v>
+        <v>0.9</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.27600000000000002</v>
+        <f>E14*1.2</f>
+        <v>1.08</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
-        <v>3.3120000000000003</v>
+        <f>A14*F14</f>
+        <v>12.96</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1">
+        <f>MAX(0, A14-G14)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="E15" s="1">
-        <v>13.21</v>
+        <v>6.35</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>15.852</v>
+        <f>E15*1.2</f>
+        <v>7.6199999999999992</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>15.852</v>
+        <f>A15*F15</f>
+        <v>15.239999999999998</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, A15-G15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>96</v>
+      <c r="A16" s="10">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>95</v>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E16" s="1">
-        <v>8.6999999999999994E-2</v>
+        <v>0.2092</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ref="F16" si="3">E16*1.2</f>
-        <v>0.10439999999999999</v>
+        <f>E16*1.2</f>
+        <v>0.25103999999999999</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
         <v>100</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16" si="4">A16*F16</f>
-        <v>1.2527999999999999</v>
+        <f>A16*F16</f>
+        <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f>MAX(0, A16-G16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>98</v>
+      <c r="D17" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E17" s="1">
-        <v>1.7</v>
+        <v>0.19</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>2.04</v>
+        <f>E17*1.2</f>
+        <v>0.22799999999999998</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
-        <v>2.04</v>
+        <f>A17*F17</f>
+        <v>0.45599999999999996</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1">
+        <f>MAX(0, A17-G17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>12</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>92</v>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>93</v>
+        <v>17</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.23499999999999999</v>
       </c>
       <c r="F18" s="1">
-        <v>0.28899999999999998</v>
+        <f>E18*1.2</f>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G18" s="1">
-        <v>12</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>3.468</v>
+        <f>A18*F18</f>
+        <v>3.3839999999999995</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1">
-      <c r="A19">
-        <v>4</v>
+        <f>MAX(0, A18-G18)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="10">
+        <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1">
-        <v>3.7</v>
+        <v>4.71</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>4.4400000000000004</v>
+        <f>E19*1.2</f>
+        <v>5.6520000000000001</v>
       </c>
       <c r="G19" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
-        <v>17.760000000000002</v>
+        <f>A19*F19</f>
+        <v>0</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
+        <f>MAX(0, A19-G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
+      <c r="D20" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="1">
-        <v>0.187</v>
+        <v>0.77</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.22439999999999999</v>
+        <f>E20*1.2</f>
+        <v>0.92399999999999993</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
-        <v>2.2439999999999998</v>
+        <f>A20*F20</f>
+        <v>1.8479999999999999</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1">
+        <f>MAX(0, A20-G20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>17</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="E21" s="1">
-        <v>25.99</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>31.187999999999995</v>
+        <f>E21*1.2</f>
+        <v>0.10439999999999999</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="I21">
-        <f t="shared" si="1"/>
-        <v>31.187999999999995</v>
+        <f>A21*F21</f>
+        <v>2.0880000000000001</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1">
+        <f>MAX(0, A21-G21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="E22" s="1">
-        <v>5</v>
+        <v>1.7</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>E22*1.2</f>
+        <v>2.04</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>A22*F22</f>
+        <v>4.08</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1">
+        <f>MAX(0, A22-G22)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="4">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1">
+        <v>8.2200000000000006</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>E23*1.2</f>
+        <v>9.8640000000000008</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f>A23*F23</f>
+        <v>9.8640000000000008</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1">
+        <f>MAX(0, A23-G23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>77</v>
+      <c r="B24" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.08</v>
       </c>
       <c r="F24" s="1">
-        <v>40.299999999999997</v>
+        <f>E24*1.2</f>
+        <v>2.496</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
-        <v>40.299999999999997</v>
+        <f>A24*F24</f>
+        <v>2.496</v>
       </c>
       <c r="J24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1">
+        <f>MAX(0, A24-G24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.31</v>
       </c>
       <c r="F25" s="1">
-        <v>3.28</v>
+        <f>E25*1.2</f>
+        <v>0.372</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
-        <v>6.56</v>
+        <f>A25*F25</f>
+        <v>0.74399999999999999</v>
       </c>
       <c r="J25">
-        <f t="shared" si="2"/>
+        <f>MAX(0, A25-G25)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:10">
       <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G26" s="1">
+        <v>12</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26">
+        <f>A26*F26</f>
+        <v>3.468</v>
+      </c>
+      <c r="J26">
+        <f>MAX(0, A26-G26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27">
+        <f>A27*F27</f>
+        <v>15</v>
+      </c>
+      <c r="J27">
+        <f>MAX(0, A27-G27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="1">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1.2</f>
+        <v>6</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3.46</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>4.1520000000000001</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
-        <v>4.1520000000000001</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="1">
-        <v>695</v>
-      </c>
-      <c r="E27" s="1">
-        <v>37.92</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>45.503999999999998</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
-        <v>45.503999999999998</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="1">
-        <v>696</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1.63</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9559999999999997</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
       <c r="I28">
-        <f t="shared" si="1"/>
-        <v>3.9119999999999995</v>
+        <f>A28*F28</f>
+        <v>6</v>
       </c>
       <c r="J28">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>MAX(0, A28-G28)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1736,383 +1848,347 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="1">
-        <v>8.2200000000000006</v>
+        <v>41</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="4">
+        <v>30</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="0"/>
-        <v>9.8640000000000008</v>
+        <f>E29*1.2</f>
+        <v>36</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
-        <v>9.8640000000000008</v>
+        <f>A29*F29</f>
+        <v>36</v>
       </c>
       <c r="J29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1">
+        <f>MAX(0, A29-G29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="4">
+        <v>8</v>
       </c>
       <c r="F30" s="1">
-        <v>4.99</v>
+        <f>E30*1.2</f>
+        <v>9.6</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30">
+        <f>A30*F30</f>
+        <v>9.6</v>
+      </c>
+      <c r="J30">
+        <f>MAX(0, A30-G30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
-        <v>4.99</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>66</v>
+      <c r="C31" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="F31" s="1">
-        <v>45.99</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
-        <v>45.99</v>
+        <f>A31*F31</f>
+        <v>40.299999999999997</v>
       </c>
       <c r="J31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>104</v>
+        <f>MAX(0, A31-G31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="10">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>34</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3.7</v>
       </c>
       <c r="F32" s="1">
-        <v>15</v>
+        <f>E32*1.2</f>
+        <v>4.4400000000000004</v>
       </c>
       <c r="G32" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>A32*F32</f>
+        <v>0</v>
       </c>
       <c r="J32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1">
+        <f>MAX(0, A32-G32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>46</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.28999999999999998</v>
       </c>
       <c r="F33" s="1">
-        <v>8.42</v>
+        <f>E33*1.2</f>
+        <v>0.34799999999999998</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
-        <v>8.42</v>
+        <f>A33*F33</f>
+        <v>5.5679999999999996</v>
       </c>
       <c r="J33">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, A33-G33)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>80</v>
+        <v>46</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="E34" s="1">
-        <v>2.08</v>
+        <v>0.23</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F35" si="5">E34*1.2</f>
-        <v>2.496</v>
+        <f>E34*1.2</f>
+        <v>0.27600000000000002</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
-        <v>2.496</v>
+        <f>A34*F34</f>
+        <v>4.4160000000000004</v>
       </c>
       <c r="J34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1">
+        <f>MAX(0, A34-G34)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>1</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>13.21</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="5"/>
+        <f>E35*1.2</f>
+        <v>15.852</v>
+      </c>
+      <c r="G35" s="1">
         <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>A35*F35</f>
+        <v>15.852</v>
       </c>
       <c r="J35">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1">
+        <f>MAX(0, A35-G35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1.2</f>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>A36*F36</f>
+        <v>1.6800000000000002</v>
       </c>
       <c r="J36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1">
+        <f>MAX(0, A36-G36)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3.46</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1.2</f>
+        <v>4.1520000000000001</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I37">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>A37*F37</f>
+        <v>4.1520000000000001</v>
       </c>
       <c r="J37">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1">
+        <f>MAX(0, A37-G37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f>A38*F38</f>
         <v>0</v>
       </c>
       <c r="J38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1">
-      <c r="I39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1">
-      <c r="I40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1">
-      <c r="I41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1">
-      <c r="I42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1">
-      <c r="I43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1">
-      <c r="I44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1">
-      <c r="I45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1">
-      <c r="I46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1">
-      <c r="I47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1">
-      <c r="I48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="9:10" hidden="1">
-      <c r="I49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="9:10" hidden="1">
-      <c r="I50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, A38-G38)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F50">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="DIGIKEY"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:J1">
+    <sortState ref="A2:J38">
+      <sortCondition ref="C1:C38"/>
+    </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1:J22 J24:J1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
@@ -2142,13 +2218,13 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
         <f>SUM(Sheet1!I:I)</f>
-        <v>568.27679999999987</v>
+        <v>538.4140000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>